<commit_message>
more papers on the xcel
</commit_message>
<xml_diff>
--- a/full text screen - MC .xlsx
+++ b/full text screen - MC .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1640" windowWidth="25120" windowHeight="13480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="full text screen - MC (referenc" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7327" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7331" uniqueCount="801">
   <si>
     <t>A1</t>
   </si>
@@ -2434,15 +2434,43 @@
   <si>
     <t>PLAGIARISMMMM!!!!1!1111!!!!</t>
   </si>
+  <si>
+    <t>a review, not enough info on data</t>
+  </si>
+  <si>
+    <t>Russian!</t>
+  </si>
+  <si>
+    <t>doesn't fit into any of the studies</t>
+  </si>
+  <si>
+    <t>none of the experiments fit into the studies, also there may be an effect of familiarisation with the tasks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2465,8 +2493,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2475,7 +2575,79 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="73">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -2803,7 +2975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2813,10 +2985,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AC1" sqref="AC1"/>
-      <selection pane="bottomLeft" activeCell="DA76" sqref="DA76"/>
+      <selection pane="bottomLeft" activeCell="CV69" sqref="CV69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23695,6 +23867,21 @@
       <c r="CW70">
         <v>515115</v>
       </c>
+      <c r="CX70">
+        <v>0</v>
+      </c>
+      <c r="CY70">
+        <v>0</v>
+      </c>
+      <c r="CZ70">
+        <v>0</v>
+      </c>
+      <c r="DA70">
+        <v>0</v>
+      </c>
+      <c r="DB70" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="71" spans="1:106">
       <c r="A71">
@@ -23994,6 +24181,9 @@
       <c r="CW71">
         <v>515141</v>
       </c>
+      <c r="DB71" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="72" spans="1:106">
       <c r="A72">
@@ -24296,6 +24486,21 @@
       <c r="CW72">
         <v>515274</v>
       </c>
+      <c r="CX72">
+        <v>0</v>
+      </c>
+      <c r="CY72">
+        <v>0</v>
+      </c>
+      <c r="CZ72">
+        <v>0</v>
+      </c>
+      <c r="DA72">
+        <v>0</v>
+      </c>
+      <c r="DB72" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="73" spans="1:106">
       <c r="A73">
@@ -24586,6 +24791,21 @@
       <c r="CW73">
         <v>516037</v>
       </c>
+      <c r="CX73">
+        <v>0</v>
+      </c>
+      <c r="CY73">
+        <v>0</v>
+      </c>
+      <c r="CZ73">
+        <v>0</v>
+      </c>
+      <c r="DA73">
+        <v>0</v>
+      </c>
+      <c r="DB73" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="74" spans="1:106">
       <c r="A74">
@@ -24876,6 +25096,18 @@
       <c r="CW74">
         <v>516321</v>
       </c>
+      <c r="CX74">
+        <v>0</v>
+      </c>
+      <c r="CY74">
+        <v>0</v>
+      </c>
+      <c r="CZ74">
+        <v>0</v>
+      </c>
+      <c r="DA74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:106">
       <c r="A75">
@@ -25166,6 +25398,18 @@
       <c r="CW75">
         <v>516776</v>
       </c>
+      <c r="CX75">
+        <v>0</v>
+      </c>
+      <c r="CY75">
+        <v>0</v>
+      </c>
+      <c r="CZ75">
+        <v>0</v>
+      </c>
+      <c r="DA75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:106">
       <c r="A76">
@@ -25460,7 +25704,7 @@
         <v>517312</v>
       </c>
       <c r="CX76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY76">
         <v>0</v>
@@ -25469,7 +25713,7 @@
         <v>0</v>
       </c>
       <c r="DA76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:106">
@@ -26991,6 +27235,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">

</xml_diff>